<commit_message>
Weekly data update (Week 5) + inventory & sales snapshots
</commit_message>
<xml_diff>
--- a/data/raw/sales/Week 5/Nexlev/other_channels.xlsx
+++ b/data/raw/sales/Week 5/Nexlev/other_channels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Laptop\D\Nitesh\Weekly Report - B2B + B2C\FastAPI\data\raw\sales\Week 4\Nexlev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Laptop\D\Nitesh\Weekly Report - B2B + B2C\FastAPI\data\raw\sales\Week 5\Nexlev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7ADFC3-4349-442C-9C92-11CB118C0F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2D48A5-BAA5-4AEA-9A29-3764D1AD9764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{00DB3424-A17B-4A18-BC6A-329A1F1119CF}"/>
   </bookViews>
@@ -2591,9 +2591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0B945F7-C092-4C8D-90BB-32200ADB80E4}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3107,6 +3105,7 @@
       <c r="E26" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F25" xr:uid="{A0B945F7-C092-4C8D-90BB-32200ADB80E4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3116,7 +3115,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="A2:B11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3455,7 +3454,7 @@
   <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4356,6 +4355,7 @@
       <c r="F72" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F26" xr:uid="{998B2A50-6942-45EF-91DE-24539BE68CC0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>